<commit_message>
now printing random AR-code on registers
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_ОГН.xlsx
+++ b/templates/ведомость_курсанты_ОГН.xlsx
@@ -17,6 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ОГН!$S$10:$S$18</definedName>
     <definedName name="EmptyRows">ОГН!$A$12</definedName>
+    <definedName name="OCRCode">ОГН!$P$3</definedName>
     <definedName name="RegisterDate">ОГН!$A$4</definedName>
     <definedName name="SoldierList">ОГН!$A$11</definedName>
     <definedName name="ИмяПодразделения">ОГН!$A$2</definedName>
@@ -385,6 +386,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -403,9 +422,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -425,21 +441,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,7 +729,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -743,44 +744,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -801,151 +802,151 @@
       <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
     </row>
     <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="20" t="s">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="20" t="s">
+      <c r="O7" s="26"/>
+      <c r="P7" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="20"/>
+      <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="21">
         <v>2</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="4">
         <v>3</v>
       </c>
@@ -1107,58 +1108,51 @@
       <c r="S16" s="11"/>
     </row>
     <row r="17" spans="1:19" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="17" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
       <c r="S17" s="12"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
       <c r="S18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="G7:J8"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="H17:P17"/>
@@ -1174,6 +1168,13 @@
     <mergeCell ref="B7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="G7:J8"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
now storing register column widths in database before printing - to aid in table recognition
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_ОГН.xlsx
+++ b/templates/ведомость_курсанты_ОГН.xlsx
@@ -215,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -310,32 +310,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -348,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,12 +335,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -385,9 +353,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -403,44 +404,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,8 +693,8 @@
   </sheetPr>
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -744,416 +709,423 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="14" t="s">
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="26"/>
-      <c r="P7" s="14" t="s">
+      <c r="O7" s="17"/>
+      <c r="P7" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="14"/>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
       <c r="D10" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H10" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I10" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J10" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K10" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L10" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M10" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N10" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O10" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P10" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="S11" s="11"/>
-    </row>
-    <row r="12" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="S12" s="11"/>
-    </row>
-    <row r="13" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="S13" s="11"/>
-    </row>
-    <row r="14" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="S14" s="11"/>
-    </row>
-    <row r="15" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="S15" s="11"/>
-    </row>
-    <row r="16" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="S16" s="11"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="S16" s="9"/>
     </row>
     <row r="17" spans="1:19" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="23" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="S17" s="12"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="S17" s="10"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="S18" s="12"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="S18" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B10:C10"/>
+  <mergeCells count="21">
+    <mergeCell ref="G7:J8"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="H17:P17"/>
     <mergeCell ref="A18:P18"/>
@@ -1169,12 +1141,6 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="G7:J8"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tweaked print margins in register templates
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_ОГН.xlsx
+++ b/templates/ведомость_курсанты_ОГН.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pronko\prj\Grader\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YUKI\3_Вирусы\Pronko_2\prj\Grader\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -353,6 +353,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -366,9 +387,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -388,24 +406,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,8 +693,8 @@
   </sheetPr>
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -709,44 +709,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -767,142 +767,142 @@
       <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
     </row>
     <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="15" t="s">
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="17"/>
-      <c r="P7" s="15" t="s">
+      <c r="O7" s="23"/>
+      <c r="P7" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="15"/>
+      <c r="P8" s="22"/>
     </row>
     <row r="9" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -961,7 +961,7 @@
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="6"/>
@@ -982,7 +982,7 @@
     <row r="12" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="29"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1001,7 +1001,7 @@
     <row r="13" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="29"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1020,7 +1020,7 @@
     <row r="14" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="29"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1039,7 +1039,7 @@
     <row r="15" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="29"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1058,7 +1058,7 @@
     <row r="16" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="29"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1075,57 +1075,51 @@
       <c r="S16" s="9"/>
     </row>
     <row r="17" spans="1:19" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="12" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
       <c r="S17" s="10"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
       <c r="S18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G7:J8"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="H17:P17"/>
     <mergeCell ref="A18:P18"/>
@@ -1141,9 +1135,15 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:J8"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
   </mergeCells>
-  <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed horizontal centering on registers
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_ОГН.xlsx
+++ b/templates/ведомость_курсанты_ОГН.xlsx
@@ -356,9 +356,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -373,39 +406,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -709,44 +709,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -767,142 +767,142 @@
       <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
     </row>
     <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="22" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="22" t="s">
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="23"/>
-      <c r="P7" s="22" t="s">
+      <c r="O7" s="18"/>
+      <c r="P7" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="22"/>
+      <c r="P8" s="16"/>
     </row>
     <row r="9" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -1075,51 +1075,56 @@
       <c r="S16" s="9"/>
     </row>
     <row r="17" spans="1:19" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="19" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
       <c r="S17" s="10"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
       <c r="S18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="H17:P17"/>
     <mergeCell ref="A18:P18"/>
@@ -1136,12 +1141,8 @@
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="G7:J8"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>